<commit_message>
Updated rates, added slope
</commit_message>
<xml_diff>
--- a/skandia-interest.xlsx
+++ b/skandia-interest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="19">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -162,11 +162,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,16 +183,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
+      <selection pane="bottomLeft" activeCell="G86" activeCellId="0" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2065,6 +2065,98 @@
         <v>3.61</v>
       </c>
     </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="D82" s="1" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="E82" s="1" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="F82" s="1" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="G82" s="1" t="n">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D83" s="1" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="E83" s="1" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="F83" s="1" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="G83" s="1" t="n">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D84" s="1" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E84" s="1" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="F84" s="1" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="G84" s="1" t="n">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="D85" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E85" s="1" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="F85" s="1" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="G85" s="1" t="n">
+        <v>4.04</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added jan and feb
</commit_message>
<xml_diff>
--- a/skandia-interest.xlsx
+++ b/skandia-interest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="19">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -187,12 +187,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G86" activeCellId="0" sqref="G86"/>
+      <selection pane="bottomLeft" activeCell="G88" activeCellId="0" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2157,6 +2157,52 @@
         <v>4.04</v>
       </c>
     </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="D86" s="1" t="n">
+        <v>5.19</v>
+      </c>
+      <c r="E86" s="1" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="F86" s="1" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="G86" s="1" t="n">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="D87" s="1" t="n">
+        <v>5.19</v>
+      </c>
+      <c r="E87" s="1" t="n">
+        <v>5.19</v>
+      </c>
+      <c r="F87" s="1" t="n">
+        <v>5.19</v>
+      </c>
+      <c r="G87" s="1" t="n">
+        <v>4.95</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated jan-feb 2023 rates
</commit_message>
<xml_diff>
--- a/skandia-interest.xlsx
+++ b/skandia-interest.xlsx
@@ -192,7 +192,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G88" activeCellId="0" sqref="G88"/>
+      <selection pane="bottomLeft" activeCell="H82" activeCellId="0" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2165,19 +2165,19 @@
         <v>18</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>4.41</v>
+        <v>3.34</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>5.19</v>
+        <v>4.12</v>
       </c>
       <c r="E86" s="1" t="n">
-        <v>5.09</v>
+        <v>3.94</v>
       </c>
       <c r="F86" s="1" t="n">
-        <v>4.94</v>
+        <v>4.19</v>
       </c>
       <c r="G86" s="1" t="n">
-        <v>4.7</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,19 +2188,19 @@
         <v>17</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>4.25</v>
+        <v>3.5</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>5.19</v>
+        <v>4.3</v>
       </c>
       <c r="E87" s="1" t="n">
-        <v>5.19</v>
+        <v>4.19</v>
       </c>
       <c r="F87" s="1" t="n">
-        <v>5.19</v>
+        <v>3.99</v>
       </c>
       <c r="G87" s="1" t="n">
-        <v>4.95</v>
+        <v>3.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2015, ordered excel file
</commit_message>
<xml_diff>
--- a/skandia-interest.xlsx
+++ b/skandia-interest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/sk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F947307B-4E3A-EE4E-BBA7-B233A65C55E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0451349D-2495-9048-8EDC-A08BC407660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="2480" windowWidth="22940" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="2480" windowWidth="26500" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="19">
   <si>
     <t>year</t>
   </si>
@@ -449,21 +449,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ101"/>
+  <dimension ref="A1:AMI109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="5.5" style="1" customWidth="1"/>
     <col min="3" max="7" width="4.83203125" style="1" customWidth="1"/>
-    <col min="8" max="1024" width="11.5" style="1"/>
+    <col min="8" max="1023" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,186 +488,186 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
-        <v>1.49</v>
+        <v>1.58</v>
       </c>
       <c r="D2" s="2">
-        <v>1.53</v>
+        <v>1.57</v>
       </c>
       <c r="E2" s="2">
-        <v>1.64</v>
+        <v>1.67</v>
       </c>
       <c r="F2" s="2">
-        <v>1.62</v>
+        <v>1.5</v>
       </c>
       <c r="G2" s="2">
-        <v>1.97</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
-        <v>1.49</v>
+        <v>1.57</v>
       </c>
       <c r="D3" s="2">
-        <v>1.52</v>
+        <v>1.56</v>
       </c>
       <c r="E3" s="2">
-        <v>1.64</v>
+        <v>1.61</v>
       </c>
       <c r="F3" s="2">
-        <v>1.63</v>
+        <v>1.53</v>
       </c>
       <c r="G3" s="2">
-        <v>1.94</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
-        <v>1.49</v>
+        <v>1.54</v>
       </c>
       <c r="D4" s="2">
-        <v>1.51</v>
+        <v>1.58</v>
       </c>
       <c r="E4" s="2">
-        <v>1.65</v>
+        <v>1.59</v>
       </c>
       <c r="F4" s="2">
-        <v>1.66</v>
+        <v>1.62</v>
       </c>
       <c r="G4" s="2">
-        <v>2.0499999999999998</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>1.49</v>
+        <v>1.54</v>
       </c>
       <c r="D5" s="2">
-        <v>1.53</v>
+        <v>1.57</v>
       </c>
       <c r="E5" s="2">
-        <v>1.62</v>
+        <v>1.74</v>
       </c>
       <c r="F5" s="2">
-        <v>1.61</v>
+        <v>1.63</v>
       </c>
       <c r="G5" s="2">
-        <v>2.0099999999999998</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>1.49</v>
+        <v>1.53</v>
       </c>
       <c r="D6" s="2">
-        <v>1.55</v>
+        <v>1.58</v>
       </c>
       <c r="E6" s="2">
-        <v>1.62</v>
+        <v>1.64</v>
       </c>
       <c r="F6" s="2">
-        <v>1.61</v>
+        <v>1.63</v>
       </c>
       <c r="G6" s="2">
-        <v>2.0499999999999998</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D7" s="2">
-        <v>1.56</v>
+        <v>1.58</v>
       </c>
       <c r="E7" s="2">
-        <v>1.62</v>
+        <v>1.64</v>
       </c>
       <c r="F7" s="2">
         <v>1.66</v>
       </c>
       <c r="G7" s="2">
-        <v>2.0499999999999998</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D8" s="2">
-        <v>1.55</v>
+        <v>1.56</v>
       </c>
       <c r="E8" s="2">
-        <v>1.64</v>
+        <v>1.66</v>
       </c>
       <c r="F8" s="2">
         <v>1.66</v>
       </c>
       <c r="G8" s="2">
-        <v>2.0499999999999998</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D9" s="2">
-        <v>1.56</v>
+        <v>1.52</v>
       </c>
       <c r="E9" s="2">
-        <v>1.69</v>
+        <v>1.67</v>
       </c>
       <c r="F9" s="2">
-        <v>1.64</v>
+        <v>1.62</v>
       </c>
       <c r="G9" s="2">
-        <v>2.0299999999999998</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -675,22 +675,22 @@
         <v>2016</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D10" s="2">
-        <v>1.59</v>
+        <v>1.48</v>
       </c>
       <c r="E10" s="2">
-        <v>1.65</v>
+        <v>1.62</v>
       </c>
       <c r="F10" s="2">
-        <v>1.66</v>
+        <v>1.63</v>
       </c>
       <c r="G10" s="2">
-        <v>1.95</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -698,22 +698,22 @@
         <v>2016</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D11" s="2">
-        <v>1.6</v>
+        <v>1.56</v>
       </c>
       <c r="E11" s="2">
-        <v>1.68</v>
+        <v>1.69</v>
       </c>
       <c r="F11" s="2">
-        <v>1.67</v>
+        <v>1.65</v>
       </c>
       <c r="G11" s="2">
-        <v>2.08</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -721,22 +721,22 @@
         <v>2016</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="D12" s="2">
-        <v>1.56</v>
+        <v>1.6</v>
       </c>
       <c r="E12" s="2">
-        <v>1.69</v>
+        <v>1.68</v>
       </c>
       <c r="F12" s="2">
-        <v>1.65</v>
+        <v>1.67</v>
       </c>
       <c r="G12" s="2">
-        <v>2.0499999999999998</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -744,206 +744,206 @@
         <v>2016</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="D13" s="2">
-        <v>1.48</v>
+        <v>1.59</v>
       </c>
       <c r="E13" s="2">
-        <v>1.62</v>
+        <v>1.65</v>
       </c>
       <c r="F13" s="2">
-        <v>1.63</v>
+        <v>1.66</v>
       </c>
       <c r="G13" s="2">
-        <v>2.0299999999999998</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="D14" s="2">
-        <v>1.62</v>
+        <v>1.56</v>
       </c>
       <c r="E14" s="2">
-        <v>1.6</v>
+        <v>1.69</v>
       </c>
       <c r="F14" s="2">
-        <v>1.59</v>
+        <v>1.64</v>
       </c>
       <c r="G14" s="2">
-        <v>2.0099999999999998</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="D15" s="2">
-        <v>1.59</v>
+        <v>1.55</v>
       </c>
       <c r="E15" s="2">
-        <v>1.56</v>
+        <v>1.64</v>
       </c>
       <c r="F15" s="2">
-        <v>1.63</v>
+        <v>1.66</v>
       </c>
       <c r="G15" s="2">
-        <v>2.04</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="D16" s="2">
         <v>1.56</v>
       </c>
       <c r="E16" s="2">
-        <v>1.63</v>
+        <v>1.62</v>
       </c>
       <c r="F16" s="2">
-        <v>1.61</v>
+        <v>1.66</v>
       </c>
       <c r="G16" s="2">
-        <v>2.02</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="D17" s="2">
-        <v>1.57</v>
+        <v>1.55</v>
       </c>
       <c r="E17" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="F17" s="2">
         <v>1.61</v>
       </c>
-      <c r="F17" s="2">
-        <v>1.59</v>
-      </c>
       <c r="G17" s="2">
-        <v>1.95</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2">
+        <v>1.49</v>
+      </c>
+      <c r="D18" s="2">
         <v>1.53</v>
       </c>
-      <c r="D18" s="2">
-        <v>1.58</v>
-      </c>
       <c r="E18" s="2">
-        <v>1.59</v>
+        <v>1.62</v>
       </c>
       <c r="F18" s="2">
-        <v>1.64</v>
+        <v>1.61</v>
       </c>
       <c r="G18" s="2">
-        <v>2.04</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2">
-        <v>1.52</v>
+        <v>1.49</v>
       </c>
       <c r="D19" s="2">
-        <v>1.57</v>
+        <v>1.51</v>
       </c>
       <c r="E19" s="2">
-        <v>1.6</v>
+        <v>1.65</v>
       </c>
       <c r="F19" s="2">
-        <v>1.61</v>
+        <v>1.66</v>
       </c>
       <c r="G19" s="2">
-        <v>2</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2">
-        <v>1.53</v>
+        <v>1.49</v>
       </c>
       <c r="D20" s="2">
-        <v>1.6</v>
+        <v>1.52</v>
       </c>
       <c r="E20" s="2">
-        <v>1.58</v>
+        <v>1.64</v>
       </c>
       <c r="F20" s="2">
         <v>1.63</v>
       </c>
       <c r="G20" s="2">
-        <v>2.02</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2">
+        <v>1.49</v>
+      </c>
+      <c r="D21" s="2">
         <v>1.53</v>
       </c>
-      <c r="D21" s="2">
-        <v>1.58</v>
-      </c>
       <c r="E21" s="2">
-        <v>1.56</v>
+        <v>1.64</v>
       </c>
       <c r="F21" s="2">
-        <v>1.61</v>
+        <v>1.62</v>
       </c>
       <c r="G21" s="2">
-        <v>1.98</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
@@ -951,22 +951,22 @@
         <v>2017</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2">
         <v>1.53</v>
       </c>
       <c r="D22" s="2">
+        <v>1.56</v>
+      </c>
+      <c r="E22" s="2">
         <v>1.6</v>
       </c>
-      <c r="E22" s="2">
-        <v>1.57</v>
-      </c>
       <c r="F22" s="2">
-        <v>1.58</v>
+        <v>1.59</v>
       </c>
       <c r="G22" s="2">
-        <v>1.99</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -974,22 +974,22 @@
         <v>2017</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2">
         <v>1.53</v>
       </c>
       <c r="D23" s="2">
-        <v>1.57</v>
+        <v>1.52</v>
       </c>
       <c r="E23" s="2">
-        <v>1.57</v>
+        <v>1.56</v>
       </c>
       <c r="F23" s="2">
-        <v>1.61</v>
+        <v>1.59</v>
       </c>
       <c r="G23" s="2">
-        <v>1.99</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -997,22 +997,22 @@
         <v>2017</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="2">
         <v>1.53</v>
       </c>
       <c r="D24" s="2">
-        <v>1.52</v>
+        <v>1.57</v>
       </c>
       <c r="E24" s="2">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="F24" s="2">
-        <v>1.59</v>
+        <v>1.61</v>
       </c>
       <c r="G24" s="2">
-        <v>2.0099999999999998</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -1020,206 +1020,206 @@
         <v>2017</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2">
         <v>1.53</v>
       </c>
       <c r="D25" s="2">
-        <v>1.56</v>
+        <v>1.6</v>
       </c>
       <c r="E25" s="2">
-        <v>1.6</v>
+        <v>1.57</v>
       </c>
       <c r="F25" s="2">
-        <v>1.59</v>
+        <v>1.58</v>
       </c>
       <c r="G25" s="2">
-        <v>1.96</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2">
-        <v>1.41</v>
+        <v>1.53</v>
       </c>
       <c r="D26" s="2">
-        <v>1.35</v>
+        <v>1.58</v>
       </c>
       <c r="E26" s="2">
-        <v>1.39</v>
+        <v>1.56</v>
       </c>
       <c r="F26" s="2">
-        <v>1.32</v>
+        <v>1.61</v>
       </c>
       <c r="G26" s="2">
-        <v>1.72</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>1.41</v>
+        <v>1.53</v>
       </c>
       <c r="D27" s="2">
-        <v>1.34</v>
+        <v>1.6</v>
       </c>
       <c r="E27" s="2">
-        <v>1.39</v>
+        <v>1.58</v>
       </c>
       <c r="F27" s="2">
-        <v>1.33</v>
+        <v>1.63</v>
       </c>
       <c r="G27" s="2">
-        <v>1.71</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2">
-        <v>1.43</v>
+        <v>1.52</v>
       </c>
       <c r="D28" s="2">
-        <v>1.34</v>
+        <v>1.57</v>
       </c>
       <c r="E28" s="2">
-        <v>1.37</v>
+        <v>1.6</v>
       </c>
       <c r="F28" s="2">
-        <v>1.31</v>
+        <v>1.61</v>
       </c>
       <c r="G28" s="2">
-        <v>1.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="2">
-        <v>1.44</v>
+        <v>1.53</v>
       </c>
       <c r="D29" s="2">
-        <v>1.42</v>
+        <v>1.58</v>
       </c>
       <c r="E29" s="2">
-        <v>1.38</v>
+        <v>1.59</v>
       </c>
       <c r="F29" s="2">
-        <v>1.3</v>
+        <v>1.64</v>
       </c>
       <c r="G29" s="2">
-        <v>1.75</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2">
-        <v>1.46</v>
+        <v>1.52</v>
       </c>
       <c r="D30" s="2">
-        <v>1.43</v>
+        <v>1.57</v>
       </c>
       <c r="E30" s="2">
-        <v>1.4</v>
+        <v>1.61</v>
       </c>
       <c r="F30" s="2">
-        <v>1.38</v>
+        <v>1.59</v>
       </c>
       <c r="G30" s="2">
-        <v>1.79</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2">
-        <v>1.49</v>
+        <v>1.52</v>
       </c>
       <c r="D31" s="2">
-        <v>1.52</v>
+        <v>1.56</v>
       </c>
       <c r="E31" s="2">
-        <v>1.46</v>
+        <v>1.63</v>
       </c>
       <c r="F31" s="2">
-        <v>1.44</v>
+        <v>1.61</v>
       </c>
       <c r="G31" s="2">
-        <v>1.86</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C32" s="2">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="D32" s="2">
-        <v>1.51</v>
+        <v>1.59</v>
       </c>
       <c r="E32" s="2">
-        <v>1.52</v>
+        <v>1.56</v>
       </c>
       <c r="F32" s="2">
-        <v>1.58</v>
+        <v>1.63</v>
       </c>
       <c r="G32" s="2">
-        <v>2.0099999999999998</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2">
         <v>1.52</v>
       </c>
       <c r="D33" s="2">
-        <v>1.56</v>
+        <v>1.62</v>
       </c>
       <c r="E33" s="2">
         <v>1.6</v>
       </c>
       <c r="F33" s="2">
-        <v>1.57</v>
+        <v>1.59</v>
       </c>
       <c r="G33" s="2">
-        <v>1.94</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
@@ -1227,19 +1227,19 @@
         <v>2018</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C34" s="2">
         <v>1.52</v>
       </c>
       <c r="D34" s="2">
-        <v>1.59</v>
+        <v>1.53</v>
       </c>
       <c r="E34" s="2">
-        <v>1.59</v>
+        <v>1.65</v>
       </c>
       <c r="F34" s="2">
-        <v>1.58</v>
+        <v>1.6</v>
       </c>
       <c r="G34" s="2">
         <v>2.02</v>
@@ -1250,22 +1250,22 @@
         <v>2018</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C35" s="2">
         <v>1.52</v>
       </c>
       <c r="D35" s="2">
-        <v>1.59</v>
+        <v>1.57</v>
       </c>
       <c r="E35" s="2">
         <v>1.59</v>
       </c>
       <c r="F35" s="2">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="G35" s="2">
-        <v>1.97</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.15">
@@ -1273,22 +1273,22 @@
         <v>2018</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="2">
         <v>1.52</v>
       </c>
       <c r="D36" s="2">
-        <v>1.57</v>
+        <v>1.59</v>
       </c>
       <c r="E36" s="2">
         <v>1.59</v>
       </c>
       <c r="F36" s="2">
-        <v>1.6</v>
+        <v>1.59</v>
       </c>
       <c r="G36" s="2">
-        <v>2</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
@@ -1296,19 +1296,19 @@
         <v>2018</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C37" s="2">
         <v>1.52</v>
       </c>
       <c r="D37" s="2">
-        <v>1.53</v>
+        <v>1.59</v>
       </c>
       <c r="E37" s="2">
-        <v>1.65</v>
+        <v>1.59</v>
       </c>
       <c r="F37" s="2">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
       <c r="G37" s="2">
         <v>2.02</v>
@@ -1316,160 +1316,160 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C38" s="2">
-        <v>1.34</v>
+        <v>1.52</v>
       </c>
       <c r="D38" s="2">
-        <v>1.49</v>
+        <v>1.56</v>
       </c>
       <c r="E38" s="2">
-        <v>1.35</v>
+        <v>1.6</v>
       </c>
       <c r="F38" s="2">
-        <v>1.41</v>
+        <v>1.57</v>
       </c>
       <c r="G38" s="2">
-        <v>1.32</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C39" s="2">
-        <v>1.33</v>
+        <v>1.5</v>
       </c>
       <c r="D39" s="2">
-        <v>1.4</v>
+        <v>1.51</v>
       </c>
       <c r="E39" s="2">
-        <v>1.29</v>
+        <v>1.52</v>
       </c>
       <c r="F39" s="2">
-        <v>1.25</v>
+        <v>1.58</v>
       </c>
       <c r="G39" s="2">
-        <v>1.2</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C40" s="2">
-        <v>1.34</v>
+        <v>1.49</v>
       </c>
       <c r="D40" s="2">
-        <v>1.32</v>
+        <v>1.52</v>
       </c>
       <c r="E40" s="2">
-        <v>1.29</v>
+        <v>1.46</v>
       </c>
       <c r="F40" s="2">
-        <v>1.21</v>
+        <v>1.44</v>
       </c>
       <c r="G40" s="2">
-        <v>1.17</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="2">
-        <v>1.34</v>
+        <v>1.46</v>
       </c>
       <c r="D41" s="2">
-        <v>1.29</v>
+        <v>1.43</v>
       </c>
       <c r="E41" s="2">
-        <v>1.23</v>
+        <v>1.4</v>
       </c>
       <c r="F41" s="2">
-        <v>1.22</v>
+        <v>1.38</v>
       </c>
       <c r="G41" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" s="2">
-        <v>1.34</v>
+        <v>1.44</v>
       </c>
       <c r="D42" s="2">
-        <v>1.34</v>
+        <v>1.42</v>
       </c>
       <c r="E42" s="2">
-        <v>1.33</v>
+        <v>1.38</v>
       </c>
       <c r="F42" s="2">
-        <v>1.21</v>
+        <v>1.3</v>
       </c>
       <c r="G42" s="2">
-        <v>1.23</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C43" s="2">
-        <v>1.35</v>
+        <v>1.43</v>
       </c>
       <c r="D43" s="2">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E43" s="2">
-        <v>1.42</v>
+        <v>1.37</v>
       </c>
       <c r="F43" s="2">
-        <v>1.34</v>
+        <v>1.31</v>
       </c>
       <c r="G43" s="2">
-        <v>1.71</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C44" s="2">
-        <v>1.35</v>
+        <v>1.41</v>
       </c>
       <c r="D44" s="2">
+        <v>1.34</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.39</v>
+      </c>
+      <c r="F44" s="2">
         <v>1.33</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1.42</v>
-      </c>
-      <c r="F44" s="2">
-        <v>1.34</v>
       </c>
       <c r="G44" s="2">
         <v>1.71</v>
@@ -1477,16 +1477,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C45" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="D45" s="2">
         <v>1.35</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1.31</v>
       </c>
       <c r="E45" s="2">
         <v>1.39</v>
@@ -1495,7 +1495,7 @@
         <v>1.32</v>
       </c>
       <c r="G45" s="2">
-        <v>1.81</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
@@ -1503,22 +1503,22 @@
         <v>2019</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C46" s="2">
-        <v>1.37</v>
+        <v>1.4</v>
       </c>
       <c r="D46" s="2">
-        <v>1.35</v>
+        <v>1.32</v>
       </c>
       <c r="E46" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="F46" s="2">
         <v>1.32</v>
       </c>
-      <c r="F46" s="2">
-        <v>1.31</v>
-      </c>
       <c r="G46" s="2">
-        <v>1.84</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
@@ -1526,22 +1526,22 @@
         <v>2019</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C47" s="2">
         <v>1.38</v>
       </c>
       <c r="D47" s="2">
-        <v>1.29</v>
+        <v>1.33</v>
       </c>
       <c r="E47" s="2">
-        <v>1.35</v>
+        <v>1.33</v>
       </c>
       <c r="F47" s="2">
-        <v>1.28</v>
+        <v>1.32</v>
       </c>
       <c r="G47" s="2">
-        <v>1.79</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
@@ -1549,22 +1549,22 @@
         <v>2019</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="2">
         <v>1.38</v>
       </c>
       <c r="D48" s="2">
-        <v>1.33</v>
+        <v>1.29</v>
       </c>
       <c r="E48" s="2">
-        <v>1.33</v>
+        <v>1.35</v>
       </c>
       <c r="F48" s="2">
-        <v>1.32</v>
+        <v>1.28</v>
       </c>
       <c r="G48" s="2">
-        <v>1.75</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.15">
@@ -1572,206 +1572,206 @@
         <v>2019</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C49" s="2">
-        <v>1.4</v>
+        <v>1.37</v>
       </c>
       <c r="D49" s="2">
+        <v>1.35</v>
+      </c>
+      <c r="E49" s="2">
         <v>1.32</v>
       </c>
-      <c r="E49" s="2">
-        <v>1.36</v>
-      </c>
       <c r="F49" s="2">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="G49" s="2">
-        <v>1.71</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C50" s="2">
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
       <c r="D50" s="2">
-        <v>1.27</v>
+        <v>1.31</v>
       </c>
       <c r="E50" s="2">
-        <v>1.25</v>
+        <v>1.39</v>
       </c>
       <c r="F50" s="2">
-        <v>1.25</v>
+        <v>1.32</v>
       </c>
       <c r="G50" s="2">
-        <v>1.2</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C51" s="2">
-        <v>1.4</v>
+        <v>1.35</v>
       </c>
       <c r="D51" s="2">
-        <v>1.38</v>
+        <v>1.33</v>
       </c>
       <c r="E51" s="2">
-        <v>1.31</v>
+        <v>1.42</v>
       </c>
       <c r="F51" s="2">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="G51" s="2">
-        <v>1.27</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C52" s="2">
-        <v>1.41</v>
+        <v>1.35</v>
       </c>
       <c r="D52" s="2">
-        <v>1.39</v>
+        <v>1.33</v>
       </c>
       <c r="E52" s="2">
-        <v>1.38</v>
+        <v>1.42</v>
       </c>
       <c r="F52" s="2">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
       <c r="G52" s="2">
-        <v>1.3</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C53" s="2">
-        <v>1.43</v>
+        <v>1.34</v>
       </c>
       <c r="D53" s="2">
-        <v>1.45</v>
+        <v>1.34</v>
       </c>
       <c r="E53" s="2">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="F53" s="2">
-        <v>1.38</v>
+        <v>1.21</v>
       </c>
       <c r="G53" s="2">
-        <v>1.31</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C54" s="2">
-        <v>1.49</v>
+        <v>1.34</v>
       </c>
       <c r="D54" s="2">
-        <v>1.68</v>
+        <v>1.29</v>
       </c>
       <c r="E54" s="2">
-        <v>1.58</v>
+        <v>1.23</v>
       </c>
       <c r="F54" s="2">
-        <v>1.51</v>
+        <v>1.22</v>
       </c>
       <c r="G54" s="2">
-        <v>1.47</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C55" s="2">
-        <v>1.51</v>
+        <v>1.34</v>
       </c>
       <c r="D55" s="2">
-        <v>1.7</v>
+        <v>1.32</v>
       </c>
       <c r="E55" s="2">
-        <v>1.66</v>
+        <v>1.29</v>
       </c>
       <c r="F55" s="2">
-        <v>1.55</v>
+        <v>1.21</v>
       </c>
       <c r="G55" s="2">
-        <v>1.45</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C56" s="2">
-        <v>1.51</v>
+        <v>1.33</v>
       </c>
       <c r="D56" s="2">
-        <v>1.66</v>
+        <v>1.4</v>
       </c>
       <c r="E56" s="2">
-        <v>1.6</v>
+        <v>1.29</v>
       </c>
       <c r="F56" s="2">
-        <v>1.52</v>
+        <v>1.25</v>
       </c>
       <c r="G56" s="2">
-        <v>1.49</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C57" s="2">
-        <v>1.5</v>
+        <v>1.34</v>
       </c>
       <c r="D57" s="2">
-        <v>1.7</v>
+        <v>1.49</v>
       </c>
       <c r="E57" s="2">
-        <v>1.61</v>
+        <v>1.35</v>
       </c>
       <c r="F57" s="2">
-        <v>1.53</v>
+        <v>1.41</v>
       </c>
       <c r="G57" s="2">
-        <v>1.48</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.15">
@@ -1779,22 +1779,22 @@
         <v>2020</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C58" s="2">
-        <v>1.51</v>
+        <v>1.33</v>
       </c>
       <c r="D58" s="2">
-        <v>1.64</v>
+        <v>1.45</v>
       </c>
       <c r="E58" s="2">
-        <v>1.5</v>
+        <v>1.44</v>
       </c>
       <c r="F58" s="2">
-        <v>1.52</v>
+        <v>1.47</v>
       </c>
       <c r="G58" s="2">
-        <v>1.5</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.15">
@@ -1802,22 +1802,22 @@
         <v>2020</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C59" s="2">
-        <v>1.52</v>
+        <v>1.51</v>
       </c>
       <c r="D59" s="2">
-        <v>1.68</v>
+        <v>1.69</v>
       </c>
       <c r="E59" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="F59" s="2">
         <v>1.54</v>
       </c>
-      <c r="F59" s="2">
-        <v>1.55</v>
-      </c>
       <c r="G59" s="2">
-        <v>1.48</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.15">
@@ -1825,22 +1825,22 @@
         <v>2020</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C60" s="2">
-        <v>1.51</v>
+        <v>1.52</v>
       </c>
       <c r="D60" s="2">
-        <v>1.69</v>
+        <v>1.68</v>
       </c>
       <c r="E60" s="2">
-        <v>1.63</v>
+        <v>1.54</v>
       </c>
       <c r="F60" s="2">
-        <v>1.54</v>
+        <v>1.55</v>
       </c>
       <c r="G60" s="2">
-        <v>1.5</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.15">
@@ -1848,206 +1848,206 @@
         <v>2020</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C61" s="2">
-        <v>1.33</v>
+        <v>1.51</v>
       </c>
       <c r="D61" s="2">
-        <v>1.45</v>
+        <v>1.64</v>
       </c>
       <c r="E61" s="2">
-        <v>1.44</v>
+        <v>1.5</v>
       </c>
       <c r="F61" s="2">
-        <v>1.47</v>
+        <v>1.52</v>
       </c>
       <c r="G61" s="2">
-        <v>1.37</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C62" s="2">
-        <v>1.23</v>
+        <v>1.5</v>
       </c>
       <c r="D62" s="2">
-        <v>1.1299999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="E62" s="2">
-        <v>1.22</v>
+        <v>1.61</v>
       </c>
       <c r="F62" s="2">
-        <v>1.3</v>
+        <v>1.53</v>
       </c>
       <c r="G62" s="2">
-        <v>1.39</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C63" s="2">
-        <v>1.23</v>
+        <v>1.51</v>
       </c>
       <c r="D63" s="2">
-        <v>1.17</v>
+        <v>1.66</v>
       </c>
       <c r="E63" s="2">
-        <v>1.24</v>
+        <v>1.6</v>
       </c>
       <c r="F63" s="2">
-        <v>1.31</v>
+        <v>1.52</v>
       </c>
       <c r="G63" s="2">
-        <v>1.4</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C64" s="2">
-        <v>1.23</v>
+        <v>1.51</v>
       </c>
       <c r="D64" s="2">
-        <v>1.24</v>
+        <v>1.7</v>
       </c>
       <c r="E64" s="2">
-        <v>1.27</v>
+        <v>1.66</v>
       </c>
       <c r="F64" s="2">
-        <v>1.34</v>
+        <v>1.55</v>
       </c>
       <c r="G64" s="2">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C65" s="2">
-        <v>1.23</v>
+        <v>1.49</v>
       </c>
       <c r="D65" s="2">
-        <v>1.24</v>
+        <v>1.68</v>
       </c>
       <c r="E65" s="2">
-        <v>1.29</v>
+        <v>1.58</v>
       </c>
       <c r="F65" s="2">
-        <v>1.35</v>
+        <v>1.51</v>
       </c>
       <c r="G65" s="2">
-        <v>1.43</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C66" s="2">
-        <v>1.23</v>
+        <v>1.43</v>
       </c>
       <c r="D66" s="2">
-        <v>1.23</v>
+        <v>1.45</v>
       </c>
       <c r="E66" s="2">
-        <v>1.25</v>
+        <v>1.32</v>
       </c>
       <c r="F66" s="2">
-        <v>1.37</v>
+        <v>1.38</v>
       </c>
       <c r="G66" s="2">
-        <v>1.45</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C67" s="2">
-        <v>1.23</v>
+        <v>1.41</v>
       </c>
       <c r="D67" s="2">
-        <v>1.21</v>
+        <v>1.39</v>
       </c>
       <c r="E67" s="2">
-        <v>1.25</v>
+        <v>1.38</v>
       </c>
       <c r="F67" s="2">
-        <v>1.41</v>
+        <v>1.37</v>
       </c>
       <c r="G67" s="2">
-        <v>1.44</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C68" s="2">
-        <v>1.23</v>
+        <v>1.4</v>
       </c>
       <c r="D68" s="2">
-        <v>1.2</v>
+        <v>1.38</v>
       </c>
       <c r="E68" s="2">
-        <v>1.17</v>
+        <v>1.31</v>
       </c>
       <c r="F68" s="2">
         <v>1.35</v>
       </c>
       <c r="G68" s="2">
-        <v>1.38</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C69" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="E69" s="2">
         <v>1.25</v>
       </c>
-      <c r="D69" s="2">
-        <v>1.21</v>
-      </c>
-      <c r="E69" s="2">
-        <v>1.1100000000000001</v>
-      </c>
       <c r="F69" s="2">
-        <v>1.3</v>
+        <v>1.25</v>
       </c>
       <c r="G69" s="2">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.15">
@@ -2055,16 +2055,16 @@
         <v>2021</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C70" s="2">
-        <v>1.27</v>
+        <v>1.3</v>
       </c>
       <c r="D70" s="2">
-        <v>1.21</v>
+        <v>1.26</v>
       </c>
       <c r="E70" s="2">
-        <v>1.0900000000000001</v>
+        <v>1.22</v>
       </c>
       <c r="F70" s="2">
         <v>1.23</v>
@@ -2078,16 +2078,16 @@
         <v>2021</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C71" s="2">
-        <v>1.26</v>
+        <v>1.29</v>
       </c>
       <c r="D71" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="E71" s="2">
         <v>1.25</v>
-      </c>
-      <c r="E71" s="2">
-        <v>1.19</v>
       </c>
       <c r="F71" s="2">
         <v>1.22</v>
@@ -2101,16 +2101,16 @@
         <v>2021</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C72" s="2">
-        <v>1.29</v>
+        <v>1.26</v>
       </c>
       <c r="D72" s="2">
-        <v>1.29</v>
+        <v>1.25</v>
       </c>
       <c r="E72" s="2">
-        <v>1.25</v>
+        <v>1.19</v>
       </c>
       <c r="F72" s="2">
         <v>1.22</v>
@@ -2124,16 +2124,16 @@
         <v>2021</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C73" s="2">
-        <v>1.3</v>
+        <v>1.27</v>
       </c>
       <c r="D73" s="2">
-        <v>1.26</v>
+        <v>1.21</v>
       </c>
       <c r="E73" s="2">
-        <v>1.22</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F73" s="2">
         <v>1.23</v>
@@ -2144,462 +2144,462 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C74" s="2">
-        <v>1.22</v>
+        <v>1.25</v>
       </c>
       <c r="D74" s="2">
-        <v>1.4</v>
+        <v>1.21</v>
       </c>
       <c r="E74" s="2">
-        <v>1.84</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="F74" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.3</v>
       </c>
       <c r="G74" s="2">
-        <v>2.4500000000000002</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C75" s="2">
-        <v>1.21</v>
+        <v>1.23</v>
       </c>
       <c r="D75" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="E75" s="2">
-        <v>1.44</v>
+        <v>1.17</v>
       </c>
       <c r="F75" s="2">
-        <v>1.72</v>
+        <v>1.35</v>
       </c>
       <c r="G75" s="2">
-        <v>2</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C76" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="D76" s="2">
         <v>1.21</v>
       </c>
-      <c r="D76" s="2">
-        <v>1.1200000000000001</v>
-      </c>
       <c r="E76" s="2">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
       <c r="F76" s="2">
         <v>1.41</v>
       </c>
       <c r="G76" s="2">
-        <v>1.65</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C77" s="2">
-        <v>1.21</v>
+        <v>1.23</v>
       </c>
       <c r="D77" s="2">
-        <v>1.1200000000000001</v>
+        <v>1.23</v>
       </c>
       <c r="E77" s="2">
-        <v>1.23</v>
+        <v>1.25</v>
       </c>
       <c r="F77" s="2">
-        <v>1.32</v>
+        <v>1.37</v>
       </c>
       <c r="G77" s="2">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
-        <v>2022</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C78" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="2">
         <v>1.23</v>
       </c>
-      <c r="D78" s="1">
-        <v>1.93</v>
-      </c>
-      <c r="E78" s="1">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="F78" s="1">
-        <v>2.83</v>
-      </c>
-      <c r="G78" s="1">
-        <v>2.93</v>
+      <c r="D78" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="F78" s="2">
+        <v>1.35</v>
+      </c>
+      <c r="G78" s="2">
+        <v>1.43</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
-        <v>2022</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="1">
-        <v>1.62</v>
-      </c>
-      <c r="D79" s="1">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="E79" s="1">
-        <v>3.04</v>
-      </c>
-      <c r="F79" s="1">
-        <v>3.3</v>
-      </c>
-      <c r="G79" s="1">
-        <v>3.34</v>
+        <v>2021</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1.34</v>
+      </c>
+      <c r="G79" s="2">
+        <v>1.43</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
-        <v>2022</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C80" s="1">
-        <v>1.97</v>
-      </c>
-      <c r="D80" s="1">
-        <v>2.88</v>
-      </c>
-      <c r="E80" s="1">
-        <v>3.51</v>
-      </c>
-      <c r="F80" s="1">
-        <v>3.72</v>
-      </c>
-      <c r="G80" s="1">
-        <v>3.78</v>
+        <v>2021</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1.17</v>
+      </c>
+      <c r="E80" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="F80" s="2">
+        <v>1.31</v>
+      </c>
+      <c r="G80" s="2">
+        <v>1.4</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
-        <v>2022</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C81" s="1">
-        <v>2.46</v>
-      </c>
-      <c r="D81" s="1">
-        <v>3.21</v>
-      </c>
-      <c r="E81" s="1">
-        <v>3.61</v>
-      </c>
-      <c r="F81" s="1">
-        <v>3.67</v>
-      </c>
-      <c r="G81" s="1">
-        <v>3.61</v>
+        <v>2021</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E81" s="2">
+        <v>1.22</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="G81" s="2">
+        <v>1.39</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>2022</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="1">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="D82" s="1">
-        <v>3.49</v>
-      </c>
-      <c r="E82" s="1">
-        <v>3.91</v>
-      </c>
-      <c r="F82" s="1">
-        <v>3.79</v>
-      </c>
-      <c r="G82" s="1">
-        <v>3.75</v>
+      <c r="B82" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E82" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="G82" s="2">
+        <v>1.43</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>2022</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="D83" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="E83" s="1">
-        <v>4.05</v>
-      </c>
-      <c r="F83" s="1">
-        <v>4.01</v>
-      </c>
-      <c r="G83" s="1">
-        <v>3.89</v>
+      <c r="B83" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1.65</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>2022</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="D84" s="1">
-        <v>3.73</v>
-      </c>
-      <c r="E84" s="1">
-        <v>4.08</v>
-      </c>
-      <c r="F84" s="1">
-        <v>4.08</v>
-      </c>
-      <c r="G84" s="1">
-        <v>3.97</v>
+      <c r="B84" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E84" s="2">
+        <v>1.44</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1.72</v>
+      </c>
+      <c r="G84" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>2022</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C85" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="D85" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="E85" s="1">
-        <v>4.07</v>
-      </c>
-      <c r="F85" s="1">
-        <v>4.05</v>
-      </c>
-      <c r="G85" s="1">
-        <v>4.04</v>
+      <c r="B85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1.22</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1.84</v>
+      </c>
+      <c r="F85" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G85" s="2">
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C86" s="1">
-        <v>3.34</v>
+        <v>1.23</v>
       </c>
       <c r="D86" s="1">
-        <v>4.12</v>
+        <v>1.93</v>
       </c>
       <c r="E86" s="1">
-        <v>3.94</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="F86" s="1">
-        <v>4.1900000000000004</v>
+        <v>2.83</v>
       </c>
       <c r="G86" s="1">
-        <v>3.48</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C87" s="1">
-        <v>3.5</v>
+        <v>1.62</v>
       </c>
       <c r="D87" s="1">
-        <v>4.3</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="E87" s="1">
-        <v>4.1900000000000004</v>
+        <v>3.04</v>
       </c>
       <c r="F87" s="1">
-        <v>3.99</v>
+        <v>3.3</v>
       </c>
       <c r="G87" s="1">
-        <v>3.91</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C88" s="1">
-        <v>3.88</v>
+        <v>1.97</v>
       </c>
       <c r="D88" s="1">
-        <v>4.6399999999999997</v>
+        <v>2.88</v>
       </c>
       <c r="E88" s="1">
-        <v>4.57</v>
+        <v>3.51</v>
       </c>
       <c r="F88" s="1">
-        <v>4.45</v>
+        <v>3.72</v>
       </c>
       <c r="G88" s="1">
-        <v>4.18</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C89" s="1">
-        <v>3.88</v>
+        <v>2.46</v>
       </c>
       <c r="D89" s="1">
-        <v>4.71</v>
+        <v>3.21</v>
       </c>
       <c r="E89" s="1">
-        <v>4.59</v>
+        <v>3.61</v>
       </c>
       <c r="F89" s="1">
-        <v>4.32</v>
+        <v>3.67</v>
       </c>
       <c r="G89" s="1">
-        <v>4.18</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C90" s="1">
-        <v>3.89</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D90" s="1">
-        <v>4.6900000000000004</v>
+        <v>3.49</v>
       </c>
       <c r="E90" s="1">
-        <v>4.58</v>
+        <v>3.91</v>
       </c>
       <c r="F90" s="1">
-        <v>4.4800000000000004</v>
+        <v>3.79</v>
       </c>
       <c r="G90" s="1">
-        <v>3.77</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C91" s="1">
-        <v>4.13</v>
+        <v>2.7</v>
       </c>
       <c r="D91" s="1">
-        <v>4.7</v>
+        <v>3.6</v>
       </c>
       <c r="E91" s="1">
-        <v>4.63</v>
+        <v>4.05</v>
       </c>
       <c r="F91" s="1">
-        <v>4.4400000000000004</v>
+        <v>4.01</v>
       </c>
       <c r="G91" s="1">
-        <v>4.38</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C92" s="1">
-        <v>4.24</v>
+        <v>2.7</v>
       </c>
       <c r="D92" s="1">
-        <v>4.79</v>
+        <v>3.73</v>
       </c>
       <c r="E92" s="1">
-        <v>4.7300000000000004</v>
+        <v>4.08</v>
       </c>
       <c r="F92" s="1">
-        <v>4.47</v>
+        <v>4.08</v>
       </c>
       <c r="G92" s="1">
-        <v>4.3</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C93" s="1">
-        <v>4.4400000000000004</v>
+        <v>3.13</v>
       </c>
       <c r="D93" s="1">
-        <v>4.92</v>
+        <v>3.8</v>
       </c>
       <c r="E93" s="1">
-        <v>4.76</v>
+        <v>4.07</v>
       </c>
       <c r="F93" s="1">
-        <v>4.42</v>
+        <v>4.05</v>
       </c>
       <c r="G93" s="1">
-        <v>4.24</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.15">
@@ -2607,22 +2607,22 @@
         <v>2023</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C94" s="1">
-        <v>4.54</v>
+        <v>3.34</v>
       </c>
       <c r="D94" s="1">
-        <v>4.97</v>
+        <v>4.12</v>
       </c>
       <c r="E94" s="1">
-        <v>4.6399999999999997</v>
+        <v>3.94</v>
       </c>
       <c r="F94" s="1">
-        <v>4.49</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="G94" s="1">
-        <v>4.26</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.15">
@@ -2630,22 +2630,22 @@
         <v>2023</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C95" s="1">
-        <v>4.54</v>
+        <v>3.5</v>
       </c>
       <c r="D95" s="1">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="E95" s="1">
-        <v>4.82</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="F95" s="1">
-        <v>4.6100000000000003</v>
+        <v>3.99</v>
       </c>
       <c r="G95" s="1">
-        <v>4.4000000000000004</v>
+        <v>3.91</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.15">
@@ -2653,22 +2653,22 @@
         <v>2023</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C96" s="1">
-        <v>4.6900000000000004</v>
+        <v>3.88</v>
       </c>
       <c r="D96" s="1">
-        <v>5</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="E96" s="1">
-        <v>4.6900000000000004</v>
+        <v>4.57</v>
       </c>
       <c r="F96" s="1">
-        <v>4.55</v>
+        <v>4.45</v>
       </c>
       <c r="G96" s="1">
-        <v>4.3600000000000003</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.15">
@@ -2676,119 +2676,306 @@
         <v>2023</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C97" s="1">
-        <v>4.68</v>
+        <v>3.88</v>
       </c>
       <c r="D97" s="1">
-        <v>5.01</v>
+        <v>4.71</v>
       </c>
       <c r="E97" s="1">
-        <v>4.5199999999999996</v>
+        <v>4.59</v>
       </c>
       <c r="F97" s="1">
-        <v>4.5199999999999996</v>
+        <v>4.32</v>
       </c>
       <c r="G97" s="1">
-        <v>4.26</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C98" s="1">
-        <v>4.68</v>
+        <v>3.89</v>
       </c>
       <c r="D98" s="1">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E98" s="1">
         <v>4.58</v>
       </c>
-      <c r="E98" s="1">
-        <v>4.28</v>
-      </c>
       <c r="F98" s="1">
-        <v>3.92</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="G98" s="1">
-        <v>3.65</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C99" s="1">
-        <v>4.68</v>
+        <v>4.13</v>
       </c>
       <c r="D99" s="1">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="E99" s="1">
-        <v>3.9</v>
+        <v>4.63</v>
       </c>
       <c r="F99" s="1">
-        <v>3.72</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="G99" s="1">
-        <v>3.52</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C100" s="1">
-        <v>4.63</v>
+        <v>4.24</v>
       </c>
       <c r="D100" s="1">
-        <v>4.4000000000000004</v>
+        <v>4.79</v>
       </c>
       <c r="E100" s="1">
-        <v>3.88</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="F100" s="1">
-        <v>3.73</v>
+        <v>4.47</v>
       </c>
       <c r="G100" s="1">
-        <v>3.63</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="1">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="D101" s="1">
+        <v>4.92</v>
+      </c>
+      <c r="E101" s="1">
+        <v>4.76</v>
+      </c>
+      <c r="F101" s="1">
+        <v>4.42</v>
+      </c>
+      <c r="G101" s="1">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A102" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="1">
+        <v>4.54</v>
+      </c>
+      <c r="D102" s="1">
+        <v>4.97</v>
+      </c>
+      <c r="E102" s="1">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="F102" s="1">
+        <v>4.49</v>
+      </c>
+      <c r="G102" s="1">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A103" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="1">
+        <v>4.54</v>
+      </c>
+      <c r="D103" s="1">
+        <v>5</v>
+      </c>
+      <c r="E103" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="F103" s="1">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="G103" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A104" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="1">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D104" s="1">
+        <v>5</v>
+      </c>
+      <c r="E104" s="1">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F104" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="G104" s="1">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A105" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="1">
+        <v>4.68</v>
+      </c>
+      <c r="D105" s="1">
+        <v>5.01</v>
+      </c>
+      <c r="E105" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="F105" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="G105" s="1">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A106" s="1">
         <v>2024</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="1">
+        <v>4.68</v>
+      </c>
+      <c r="D106" s="1">
+        <v>4.58</v>
+      </c>
+      <c r="E106" s="1">
+        <v>4.28</v>
+      </c>
+      <c r="F106" s="1">
+        <v>3.92</v>
+      </c>
+      <c r="G106" s="1">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A107" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="1">
+        <v>4.68</v>
+      </c>
+      <c r="D107" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E107" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="F107" s="1">
+        <v>3.72</v>
+      </c>
+      <c r="G107" s="1">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A108" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" s="1">
+        <v>4.63</v>
+      </c>
+      <c r="D108" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E108" s="1">
+        <v>3.88</v>
+      </c>
+      <c r="F108" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="G108" s="1">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A109" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C109" s="1">
         <v>4.63</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D109" s="1">
         <v>4.3099999999999996</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E109" s="1">
         <v>3.8</v>
       </c>
-      <c r="F101" s="1">
+      <c r="F109" s="1">
         <v>3.61</v>
       </c>
-      <c r="G101" s="1">
+      <c r="G109" s="1">
         <v>3.35</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AMI109">
+    <sortCondition ref="A2:A109"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C2:G97">
+  <conditionalFormatting sqref="C10:G105">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2800,7 +2987,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C98:G101">
+  <conditionalFormatting sqref="C106:G109">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Corrected rates for last 3 months
</commit_message>
<xml_diff>
--- a/skandia-interest.xlsx
+++ b/skandia-interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/sk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F21C0E2-63B6-F542-80B4-FCC9C71356AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C0BD6A-1E7D-C044-8E91-FF16F441A823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="7160" windowWidth="25020" windowHeight="20680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19020" yWindow="1960" windowWidth="25300" windowHeight="20640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F120" sqref="F120"/>
+      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3030,19 +3030,19 @@
         <v>12</v>
       </c>
       <c r="C112" s="1">
-        <v>5.24</v>
+        <v>4.33</v>
       </c>
       <c r="D112" s="1">
-        <v>4.8600000000000003</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="E112" s="1">
-        <v>4.55</v>
+        <v>3.86</v>
       </c>
       <c r="F112" s="1">
-        <v>4.42</v>
+        <v>3.76</v>
       </c>
       <c r="G112" s="1">
-        <v>4.3499999999999996</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.15">
@@ -3053,19 +3053,19 @@
         <v>11</v>
       </c>
       <c r="C113" s="1">
-        <v>4.99</v>
+        <v>4.32</v>
       </c>
       <c r="D113" s="1">
-        <v>4.6100000000000003</v>
+        <v>3.87</v>
       </c>
       <c r="E113" s="1">
-        <v>4.3</v>
+        <v>3.59</v>
       </c>
       <c r="F113" s="1">
-        <v>4.17</v>
+        <v>3.54</v>
       </c>
       <c r="G113" s="1">
-        <v>4.0999999999999996</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.15">
@@ -3076,19 +3076,19 @@
         <v>10</v>
       </c>
       <c r="C114" s="1">
-        <v>4.82</v>
+        <v>4.08</v>
       </c>
       <c r="D114" s="1">
-        <v>4.3600000000000003</v>
+        <v>3.74</v>
       </c>
       <c r="E114" s="1">
-        <v>4.05</v>
+        <v>3.31</v>
       </c>
       <c r="F114" s="1">
-        <v>3.97</v>
+        <v>3.28</v>
       </c>
       <c r="G114" s="1">
-        <v>3.95</v>
+        <v>3.17</v>
       </c>
     </row>
   </sheetData>
@@ -3097,6 +3097,18 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C10:G105">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106:G109">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3108,7 +3120,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C106:G109">
+  <conditionalFormatting sqref="C110:G110">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3120,7 +3132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C110:G110">
+  <conditionalFormatting sqref="C111:G111">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3132,7 +3144,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C111:G111">
+  <conditionalFormatting sqref="C112:G112">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3144,7 +3156,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C112:G112">
+  <conditionalFormatting sqref="C113:G113">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3156,7 +3168,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C113:G113">
+  <conditionalFormatting sqref="C114:G114">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3168,7 +3180,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C114:G114">
+  <conditionalFormatting sqref="C115:G115">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added Jan 2025, CBPR, CBLR
</commit_message>
<xml_diff>
--- a/skandia-interest.xlsx
+++ b/skandia-interest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/sk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1E92F0-64D3-B741-A1E6-E5C119D895E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4EF982-B8A4-834E-9FE9-5AFBBD3C76CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2860" windowWidth="33840" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="4700" windowWidth="23080" windowHeight="17420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="22">
   <si>
     <t>year</t>
   </si>
   <si>
     <t>month</t>
-  </si>
-  <si>
-    <t>y0.5</t>
   </si>
   <si>
     <t>y1</t>
@@ -83,6 +80,18 @@
   <si>
     <t>Jan</t>
   </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>y0</t>
+  </si>
+  <si>
+    <t>cbpr</t>
+  </si>
+  <si>
+    <t>cblr</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -138,6 +147,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,21 +462,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI117"/>
+  <dimension ref="A1:AMH118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="5.5" style="3" customWidth="1"/>
     <col min="3" max="7" width="4.83203125" style="1" customWidth="1"/>
-    <col min="8" max="1023" width="11.5" style="1"/>
+    <col min="8" max="1022" width="11.5" style="1"/>
+    <col min="1023" max="16384" width="11.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,27 +485,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>2015</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>1.58</v>
@@ -511,13 +528,19 @@
       <c r="G2" s="2">
         <v>1.77</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2015</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>1.57</v>
@@ -534,13 +557,19 @@
       <c r="G3" s="2">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H3" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2015</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>1.54</v>
@@ -557,13 +586,19 @@
       <c r="G4" s="2">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H4" s="1">
+        <v>-0.32826</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.42174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2015</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <v>1.54</v>
@@ -580,13 +615,19 @@
       <c r="G5" s="2">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H5" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2015</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
         <v>1.53</v>
@@ -603,13 +644,19 @@
       <c r="G6" s="2">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H6" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>2015</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>1.5</v>
@@ -626,13 +673,19 @@
       <c r="G7" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H7" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>2015</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>1.5</v>
@@ -649,13 +702,19 @@
       <c r="G8" s="2">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H8" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>2015</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
         <v>1.5</v>
@@ -672,13 +731,19 @@
       <c r="G9" s="2">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H9" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2016</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2">
         <v>1.5</v>
@@ -695,13 +760,19 @@
       <c r="G10" s="2">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H10" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>2016</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>1.5</v>
@@ -718,13 +789,19 @@
       <c r="G11" s="2">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H11" s="1">
+        <v>-0.41428999999999999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.33571000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2016</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>1.49</v>
@@ -741,13 +818,19 @@
       <c r="G12" s="2">
         <v>2.08</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H12" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>2016</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
         <v>1.49</v>
@@ -764,13 +847,19 @@
       <c r="G13" s="2">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H13" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>2016</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <v>1.49</v>
@@ -787,13 +876,19 @@
       <c r="G14" s="2">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H14" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>2016</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
         <v>1.49</v>
@@ -810,13 +905,19 @@
       <c r="G15" s="2">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H15" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>2016</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2">
         <v>1.49</v>
@@ -833,13 +934,19 @@
       <c r="G16" s="2">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H16" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>2016</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <v>1.49</v>
@@ -856,13 +963,19 @@
       <c r="G17" s="2">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H17" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>2016</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2">
         <v>1.49</v>
@@ -879,13 +992,19 @@
       <c r="G18" s="2">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H18" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>2016</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2">
         <v>1.49</v>
@@ -902,13 +1021,19 @@
       <c r="G19" s="2">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H19" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>2016</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2">
         <v>1.49</v>
@@ -925,13 +1050,19 @@
       <c r="G20" s="2">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H20" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>2016</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2">
         <v>1.49</v>
@@ -948,13 +1079,19 @@
       <c r="G21" s="2">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H21" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>2017</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2">
         <v>1.53</v>
@@ -971,13 +1108,19 @@
       <c r="G22" s="2">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H22" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>2017</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2">
         <v>1.53</v>
@@ -994,13 +1137,19 @@
       <c r="G23" s="2">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H23" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>2017</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2">
         <v>1.53</v>
@@ -1017,13 +1166,19 @@
       <c r="G24" s="2">
         <v>1.99</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H24" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>2017</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="2">
         <v>1.53</v>
@@ -1040,13 +1195,19 @@
       <c r="G25" s="2">
         <v>1.99</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H25" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>2017</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="2">
         <v>1.53</v>
@@ -1063,13 +1224,19 @@
       <c r="G26" s="2">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H26" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>2017</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2">
         <v>1.53</v>
@@ -1086,13 +1253,19 @@
       <c r="G27" s="2">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H27" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>2017</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2">
         <v>1.52</v>
@@ -1109,13 +1282,19 @@
       <c r="G28" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H28" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>2017</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" s="2">
         <v>1.53</v>
@@ -1132,13 +1311,19 @@
       <c r="G29" s="2">
         <v>2.04</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H29" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>2017</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2">
         <v>1.52</v>
@@ -1155,13 +1340,19 @@
       <c r="G30" s="2">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H30" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>2017</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="2">
         <v>1.52</v>
@@ -1178,13 +1369,19 @@
       <c r="G31" s="2">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H31" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>2017</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2">
         <v>1.52</v>
@@ -1201,13 +1398,19 @@
       <c r="G32" s="2">
         <v>2.04</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H32" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>2017</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2">
         <v>1.52</v>
@@ -1224,13 +1427,19 @@
       <c r="G33" s="2">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H33" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>2018</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="2">
         <v>1.52</v>
@@ -1247,13 +1456,19 @@
       <c r="G34" s="2">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H34" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>2018</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="2">
         <v>1.52</v>
@@ -1270,13 +1485,19 @@
       <c r="G35" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H35" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>2018</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36" s="2">
         <v>1.52</v>
@@ -1293,13 +1514,19 @@
       <c r="G36" s="2">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H36" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>2018</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37" s="2">
         <v>1.52</v>
@@ -1316,13 +1543,19 @@
       <c r="G37" s="2">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H37" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>2018</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C38" s="2">
         <v>1.52</v>
@@ -1339,13 +1572,19 @@
       <c r="G38" s="2">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H38" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>2018</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39" s="2">
         <v>1.5</v>
@@ -1362,13 +1601,19 @@
       <c r="G39" s="2">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H39" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>2018</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40" s="2">
         <v>1.49</v>
@@ -1385,13 +1630,19 @@
       <c r="G40" s="2">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H40" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>2018</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="2">
         <v>1.46</v>
@@ -1408,13 +1659,19 @@
       <c r="G41" s="2">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H41" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>2018</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="2">
         <v>1.44</v>
@@ -1431,13 +1688,19 @@
       <c r="G42" s="2">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H42" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>2018</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" s="2">
         <v>1.43</v>
@@ -1454,13 +1717,19 @@
       <c r="G43" s="2">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H43" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
         <v>2018</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="2">
         <v>1.41</v>
@@ -1477,13 +1746,19 @@
       <c r="G44" s="2">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H44" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>2018</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2">
         <v>1.41</v>
@@ -1500,13 +1775,19 @@
       <c r="G45" s="2">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H45" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
         <v>2019</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="2">
         <v>1.4</v>
@@ -1523,13 +1804,19 @@
       <c r="G46" s="2">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H46" s="1">
+        <v>-0.30681999999999998</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.44318000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
         <v>2019</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C47" s="2">
         <v>1.38</v>
@@ -1546,13 +1833,19 @@
       <c r="G47" s="2">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H47" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
         <v>2019</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C48" s="2">
         <v>1.38</v>
@@ -1569,13 +1862,19 @@
       <c r="G48" s="2">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H48" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>2019</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C49" s="2">
         <v>1.37</v>
@@ -1592,13 +1891,19 @@
       <c r="G49" s="2">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H49" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>2019</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50" s="2">
         <v>1.35</v>
@@ -1615,13 +1920,19 @@
       <c r="G50" s="2">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H50" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>2019</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C51" s="2">
         <v>1.35</v>
@@ -1638,13 +1949,19 @@
       <c r="G51" s="2">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H51" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>2019</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" s="2">
         <v>1.35</v>
@@ -1661,13 +1978,19 @@
       <c r="G52" s="2">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H52" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>2019</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C53" s="2">
         <v>1.34</v>
@@ -1684,13 +2007,19 @@
       <c r="G53" s="2">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H53" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>2019</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C54" s="2">
         <v>1.34</v>
@@ -1707,13 +2036,19 @@
       <c r="G54" s="2">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H54" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>2019</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" s="2">
         <v>1.34</v>
@@ -1730,13 +2065,19 @@
       <c r="G55" s="2">
         <v>1.17</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H55" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>2019</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="2">
         <v>1.33</v>
@@ -1753,13 +2094,19 @@
       <c r="G56" s="2">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H56" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>2019</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" s="2">
         <v>1.34</v>
@@ -1776,13 +2123,19 @@
       <c r="G57" s="2">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H57" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58" s="3">
         <v>2020</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" s="2">
         <v>1.33</v>
@@ -1799,13 +2152,19 @@
       <c r="G58" s="2">
         <v>1.37</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H58" s="1">
+        <v>-3.5714000000000003E-2</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0.71428999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
         <v>2020</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C59" s="2">
         <v>1.51</v>
@@ -1822,13 +2181,19 @@
       <c r="G59" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A60" s="3">
         <v>2020</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C60" s="2">
         <v>1.52</v>
@@ -1845,13 +2210,19 @@
       <c r="G60" s="2">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61" s="3">
         <v>2020</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C61" s="2">
         <v>1.51</v>
@@ -1868,13 +2239,19 @@
       <c r="G61" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62" s="3">
         <v>2020</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="2">
         <v>1.5</v>
@@ -1891,13 +2268,19 @@
       <c r="G62" s="2">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A63" s="3">
         <v>2020</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" s="2">
         <v>1.51</v>
@@ -1914,13 +2297,19 @@
       <c r="G63" s="2">
         <v>1.49</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64" s="3">
         <v>2020</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C64" s="2">
         <v>1.51</v>
@@ -1937,13 +2326,19 @@
       <c r="G64" s="2">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0.10435</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" s="3">
         <v>2020</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C65" s="2">
         <v>1.49</v>
@@ -1960,13 +2355,19 @@
       <c r="G65" s="2">
         <v>1.47</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="3">
         <v>2020</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66" s="2">
         <v>1.43</v>
@@ -1983,13 +2384,19 @@
       <c r="G66" s="2">
         <v>1.31</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A67" s="3">
         <v>2020</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67" s="2">
         <v>1.41</v>
@@ -2006,13 +2413,19 @@
       <c r="G67" s="2">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A68" s="3">
         <v>2020</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68" s="2">
         <v>1.4</v>
@@ -2029,13 +2442,19 @@
       <c r="G68" s="2">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A69" s="3">
         <v>2020</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" s="2">
         <v>1.3</v>
@@ -2052,13 +2471,19 @@
       <c r="G69" s="2">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A70" s="3">
         <v>2021</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70" s="2">
         <v>1.3</v>
@@ -2075,13 +2500,19 @@
       <c r="G70" s="2">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A71" s="3">
         <v>2021</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C71" s="2">
         <v>1.29</v>
@@ -2098,13 +2529,19 @@
       <c r="G71" s="2">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A72" s="3">
         <v>2021</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C72" s="2">
         <v>1.26</v>
@@ -2121,13 +2558,19 @@
       <c r="G72" s="2">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A73" s="3">
         <v>2021</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C73" s="2">
         <v>1.27</v>
@@ -2144,13 +2587,19 @@
       <c r="G73" s="2">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H73" s="1">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A74" s="3">
         <v>2021</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C74" s="2">
         <v>1.25</v>
@@ -2167,13 +2616,19 @@
       <c r="G74" s="2">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H74" s="1">
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75" s="3">
         <v>2021</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C75" s="2">
         <v>1.23</v>
@@ -2190,13 +2645,19 @@
       <c r="G75" s="2">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="3">
         <v>2021</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C76" s="2">
         <v>1.23</v>
@@ -2213,13 +2674,19 @@
       <c r="G76" s="2">
         <v>1.44</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A77" s="3">
         <v>2021</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C77" s="2">
         <v>1.23</v>
@@ -2236,13 +2703,19 @@
       <c r="G77" s="2">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A78" s="3">
         <v>2021</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C78" s="2">
         <v>1.23</v>
@@ -2259,13 +2732,19 @@
       <c r="G78" s="2">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
         <v>2021</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79" s="2">
         <v>1.23</v>
@@ -2282,13 +2761,19 @@
       <c r="G79" s="2">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
         <v>2021</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C80" s="2">
         <v>1.23</v>
@@ -2305,13 +2790,19 @@
       <c r="G80" s="2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
         <v>2021</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81" s="2">
         <v>1.23</v>
@@ -2328,13 +2819,19 @@
       <c r="G81" s="2">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
         <v>2022</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C82" s="2">
         <v>1.21</v>
@@ -2351,13 +2848,19 @@
       <c r="G82" s="2">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H82" s="1">
+        <v>0</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
         <v>2022</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C83" s="2">
         <v>1.21</v>
@@ -2374,13 +2877,19 @@
       <c r="G83" s="2">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H83" s="1">
+        <v>0</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>2022</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C84" s="2">
         <v>1.21</v>
@@ -2397,13 +2906,19 @@
       <c r="G84" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A85" s="3">
         <v>2022</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C85" s="2">
         <v>1.22</v>
@@ -2420,13 +2935,19 @@
       <c r="G85" s="2">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>2022</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C86" s="1">
         <v>1.23</v>
@@ -2443,13 +2964,19 @@
       <c r="G86" s="1">
         <v>2.93</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H86" s="1">
+        <v>0.22619</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0.32618999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>2022</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C87" s="1">
         <v>1.62</v>
@@ -2466,13 +2993,19 @@
       <c r="G87" s="1">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H87" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
         <v>2022</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C88" s="1">
         <v>1.97</v>
@@ -2489,13 +3022,19 @@
       <c r="G88" s="1">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H88" s="1">
+        <v>0.67857000000000001</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0.77856999999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>2022</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1">
         <v>2.46</v>
@@ -2512,13 +3051,19 @@
       <c r="G89" s="1">
         <v>3.61</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H89" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>2022</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C90" s="1">
         <v>2.4700000000000002</v>
@@ -2535,13 +3080,19 @@
       <c r="G90" s="1">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H90" s="1">
+        <v>1.11364</v>
+      </c>
+      <c r="I90" s="1">
+        <v>1.2136400000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>2022</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91" s="1">
         <v>2.7</v>
@@ -2558,13 +3109,19 @@
       <c r="G91" s="1">
         <v>3.89</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H91" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="I91" s="1">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
         <v>2022</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C92" s="1">
         <v>2.7</v>
@@ -2581,13 +3138,19 @@
       <c r="G92" s="1">
         <v>3.97</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H92" s="1">
+        <v>1.78409</v>
+      </c>
+      <c r="I92" s="1">
+        <v>1.88409</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A93" s="3">
         <v>2022</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93" s="1">
         <v>3.13</v>
@@ -2604,13 +3167,19 @@
       <c r="G93" s="1">
         <v>4.04</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H93" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I93" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
         <v>2023</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C94" s="1">
         <v>3.34</v>
@@ -2627,13 +3196,19 @@
       <c r="G94" s="1">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H94" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I94" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
         <v>2023</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C95" s="1">
         <v>3.5</v>
@@ -2650,13 +3225,19 @@
       <c r="G95" s="1">
         <v>3.91</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H95" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="I95" s="1">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A96" s="3">
         <v>2023</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C96" s="1">
         <v>3.88</v>
@@ -2673,13 +3254,19 @@
       <c r="G96" s="1">
         <v>4.18</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H96" s="1">
+        <v>3</v>
+      </c>
+      <c r="I96" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A97" s="3">
         <v>2023</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C97" s="1">
         <v>3.88</v>
@@ -2696,13 +3283,19 @@
       <c r="G97" s="1">
         <v>4.18</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H97" s="1">
+        <v>3</v>
+      </c>
+      <c r="I97" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A98" s="3">
         <v>2023</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C98" s="1">
         <v>3.89</v>
@@ -2719,13 +3312,19 @@
       <c r="G98" s="1">
         <v>3.77</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H98" s="1">
+        <v>3.4761899999999999</v>
+      </c>
+      <c r="I98" s="1">
+        <v>3.57619</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A99" s="3">
         <v>2023</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99" s="1">
         <v>4.13</v>
@@ -2742,13 +3341,19 @@
       <c r="G99" s="1">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H99" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I99" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A100" s="3">
         <v>2023</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C100" s="1">
         <v>4.24</v>
@@ -2765,13 +3370,19 @@
       <c r="G100" s="1">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H100" s="1">
+        <v>3.7261899999999999</v>
+      </c>
+      <c r="I100" s="1">
+        <v>3.82619</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A101" s="3">
         <v>2023</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C101" s="1">
         <v>4.4400000000000004</v>
@@ -2788,13 +3399,19 @@
       <c r="G101" s="1">
         <v>4.24</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H101" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I101" s="1">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A102" s="3">
         <v>2023</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C102" s="1">
         <v>4.54</v>
@@ -2811,13 +3428,19 @@
       <c r="G102" s="1">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H102" s="1">
+        <v>3.7857099999999999</v>
+      </c>
+      <c r="I102" s="1">
+        <v>3.88571</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A103" s="3">
         <v>2023</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C103" s="1">
         <v>4.54</v>
@@ -2834,13 +3457,19 @@
       <c r="G103" s="1">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H103" s="1">
+        <v>4</v>
+      </c>
+      <c r="I103" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A104" s="3">
         <v>2023</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C104" s="1">
         <v>4.6900000000000004</v>
@@ -2857,13 +3486,19 @@
       <c r="G104" s="1">
         <v>4.3600000000000003</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H104" s="1">
+        <v>4</v>
+      </c>
+      <c r="I104" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A105" s="3">
         <v>2023</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C105" s="1">
         <v>4.68</v>
@@ -2880,13 +3515,19 @@
       <c r="G105" s="1">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H105" s="1">
+        <v>4</v>
+      </c>
+      <c r="I105" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A106" s="3">
         <v>2024</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C106" s="1">
         <v>4.68</v>
@@ -2903,13 +3544,19 @@
       <c r="G106" s="1">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H106" s="1">
+        <v>4</v>
+      </c>
+      <c r="I106" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A107" s="3">
         <v>2024</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C107" s="1">
         <v>4.68</v>
@@ -2926,13 +3573,19 @@
       <c r="G107" s="1">
         <v>3.52</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H107" s="1">
+        <v>4</v>
+      </c>
+      <c r="I107" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A108" s="3">
         <v>2024</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C108" s="1">
         <v>4.63</v>
@@ -2949,13 +3602,19 @@
       <c r="G108" s="1">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H108" s="1">
+        <v>4</v>
+      </c>
+      <c r="I108" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A109" s="3">
         <v>2024</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C109" s="1">
         <v>4.63</v>
@@ -2972,13 +3631,19 @@
       <c r="G109" s="1">
         <v>3.35</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H109" s="1">
+        <v>4</v>
+      </c>
+      <c r="I109" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A110" s="3">
         <v>2024</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C110" s="1">
         <v>4.62</v>
@@ -2995,13 +3660,19 @@
       <c r="G110" s="1">
         <v>3.41</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H110" s="1">
+        <v>3.84524</v>
+      </c>
+      <c r="I110" s="1">
+        <v>3.9452400000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A111" s="3">
         <v>2024</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C111" s="1">
         <v>4.43</v>
@@ -3018,13 +3689,19 @@
       <c r="G111" s="1">
         <v>3.58</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H111" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I111" s="1">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A112" s="3">
         <v>2024</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C112" s="1">
         <v>4.33</v>
@@ -3041,13 +3718,19 @@
       <c r="G112" s="1">
         <v>3.51</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H112" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I112" s="1">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A113" s="3">
         <v>2024</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C113" s="1">
         <v>4.32</v>
@@ -3064,13 +3747,19 @@
       <c r="G113" s="1">
         <v>3.17</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H113" s="1">
+        <v>3.65909</v>
+      </c>
+      <c r="I113" s="1">
+        <v>3.75909</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A114" s="3">
         <v>2024</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C114" s="1">
         <v>4.08</v>
@@ -3087,13 +3776,19 @@
       <c r="G114" s="1">
         <v>3.17</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H114" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I114" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A115" s="3">
         <v>2024</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C115" s="1">
         <v>3.9</v>
@@ -3110,13 +3805,19 @@
       <c r="G115" s="1">
         <v>2.95</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H115" s="1">
+        <v>3.2608700000000002</v>
+      </c>
+      <c r="I115" s="1">
+        <v>3.3608699999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A116" s="3">
         <v>2024</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C116" s="1">
         <v>3.73</v>
@@ -3133,13 +3834,19 @@
       <c r="G116" s="1">
         <v>2.97</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H116" s="1">
+        <v>2.94048</v>
+      </c>
+      <c r="I116" s="1">
+        <v>3.0404800000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A117" s="3">
         <v>2024</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C117" s="1">
         <v>3.41</v>
@@ -3156,13 +3863,60 @@
       <c r="G117" s="1">
         <v>2.95</v>
       </c>
+      <c r="H117" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="I117" s="1">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A118" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118" s="1">
+        <v>3.24</v>
+      </c>
+      <c r="D118" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="E118" s="1">
+        <v>2.94</v>
+      </c>
+      <c r="F118" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="G118" s="1">
+        <v>3</v>
+      </c>
+      <c r="H118" s="1">
+        <v>2.5357099999999999</v>
+      </c>
+      <c r="I118" s="1">
+        <v>2.63571</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AMI109">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AMH109">
     <sortCondition ref="A2:A109"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C10:G105">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106:G109">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3174,7 +3928,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C106:G109">
+  <conditionalFormatting sqref="C110:G110">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3186,7 +3940,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C110:G110">
+  <conditionalFormatting sqref="C111:G111">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3198,7 +3952,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C111:G111">
+  <conditionalFormatting sqref="C112:G112">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3210,7 +3964,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C112:G112">
+  <conditionalFormatting sqref="C113:G113">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3222,7 +3976,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C113:G113">
+  <conditionalFormatting sqref="C114:G114">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3234,7 +3988,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C114:G114">
+  <conditionalFormatting sqref="C115:G115">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3246,7 +4000,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C115:G115">
+  <conditionalFormatting sqref="C116:G116">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3258,7 +4012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C116:G116">
+  <conditionalFormatting sqref="C117:G117">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3270,7 +4024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C117:G117">
+  <conditionalFormatting sqref="C118:G118">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>